<commit_message>
upgrade working work flow
</commit_message>
<xml_diff>
--- a/Documents/DFU_Summary/WAUSI_Summary_latest.xlsx
+++ b/Documents/DFU_Summary/WAUSI_Summary_latest.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="training_site_summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="training_subject_summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="validation_site_summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="validation_subject_summary" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="training_site_summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="training_subject_summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="validation_site_summary" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="validation_subject_summary" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -502,10 +502,10 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>788</v>
+        <v>869</v>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
@@ -592,10 +592,10 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>4563</v>
+        <v>4644</v>
       </c>
       <c r="D8" s="3" t="n"/>
     </row>
@@ -610,7 +610,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:B171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1293,507 +1293,507 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>203-001</t>
+          <t>202-040</t>
         </is>
       </c>
       <c r="B68" s="3" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>203-002</t>
+          <t>202-041</t>
         </is>
       </c>
       <c r="B69" s="3" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>203-003</t>
+          <t>202-042</t>
         </is>
       </c>
       <c r="B70" s="3" t="n">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>203-004</t>
+          <t>202-043</t>
         </is>
       </c>
       <c r="B71" s="3" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>203-005</t>
+          <t>202-044</t>
         </is>
       </c>
       <c r="B72" s="3" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>203-006</t>
+          <t>202-045</t>
         </is>
       </c>
       <c r="B73" s="3" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>203-007</t>
+          <t>202-046</t>
         </is>
       </c>
       <c r="B74" s="3" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>203-008</t>
+          <t>202-047</t>
         </is>
       </c>
       <c r="B75" s="3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>203-009</t>
+          <t>202-048</t>
         </is>
       </c>
       <c r="B76" s="3" t="n">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>203-010</t>
+          <t>202-049</t>
         </is>
       </c>
       <c r="B77" s="3" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>203-011</t>
+          <t>202-050</t>
         </is>
       </c>
       <c r="B78" s="3" t="n">
-        <v>46</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>203-012</t>
+          <t>202-051</t>
         </is>
       </c>
       <c r="B79" s="3" t="n">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>203-013</t>
+          <t>202-052</t>
         </is>
       </c>
       <c r="B80" s="3" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>203-014</t>
+          <t>202-053</t>
         </is>
       </c>
       <c r="B81" s="3" t="n">
-        <v>51</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>203-015</t>
+          <t>202-054</t>
         </is>
       </c>
       <c r="B82" s="3" t="n">
-        <v>67</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>203-016</t>
+          <t>202-055</t>
         </is>
       </c>
       <c r="B83" s="3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>203-017</t>
+          <t>202-056</t>
         </is>
       </c>
       <c r="B84" s="3" t="n">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>203-018</t>
+          <t>202-057</t>
         </is>
       </c>
       <c r="B85" s="3" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>203-019</t>
+          <t>202-058</t>
         </is>
       </c>
       <c r="B86" s="3" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>203-020</t>
+          <t>202-059</t>
         </is>
       </c>
       <c r="B87" s="3" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>203-021</t>
+          <t>203-001</t>
         </is>
       </c>
       <c r="B88" s="3" t="n">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>203-022</t>
+          <t>203-002</t>
         </is>
       </c>
       <c r="B89" s="3" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>203-023</t>
+          <t>203-003</t>
         </is>
       </c>
       <c r="B90" s="3" t="n">
-        <v>14</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>203-024</t>
+          <t>203-004</t>
         </is>
       </c>
       <c r="B91" s="3" t="n">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>203-025</t>
+          <t>203-005</t>
         </is>
       </c>
       <c r="B92" s="3" t="n">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>203-026</t>
+          <t>203-006</t>
         </is>
       </c>
       <c r="B93" s="3" t="n">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>203-027</t>
+          <t>203-007</t>
         </is>
       </c>
       <c r="B94" s="3" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>203-028</t>
+          <t>203-008</t>
         </is>
       </c>
       <c r="B95" s="3" t="n">
-        <v>49</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>203-029</t>
+          <t>203-009</t>
         </is>
       </c>
       <c r="B96" s="3" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>203-030</t>
+          <t>203-010</t>
         </is>
       </c>
       <c r="B97" s="3" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>203-031</t>
+          <t>203-011</t>
         </is>
       </c>
       <c r="B98" s="3" t="n">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>203-032</t>
+          <t>203-012</t>
         </is>
       </c>
       <c r="B99" s="3" t="n">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>203-033</t>
+          <t>203-013</t>
         </is>
       </c>
       <c r="B100" s="3" t="n">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>203-034</t>
+          <t>203-014</t>
         </is>
       </c>
       <c r="B101" s="3" t="n">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>203-035</t>
+          <t>203-015</t>
         </is>
       </c>
       <c r="B102" s="3" t="n">
-        <v>6</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>203-036</t>
+          <t>203-016</t>
         </is>
       </c>
       <c r="B103" s="3" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>203-037</t>
+          <t>203-017</t>
         </is>
       </c>
       <c r="B104" s="3" t="n">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>203-038</t>
+          <t>203-018</t>
         </is>
       </c>
       <c r="B105" s="3" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>203-039</t>
+          <t>203-019</t>
         </is>
       </c>
       <c r="B106" s="3" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>203-040</t>
+          <t>203-020</t>
         </is>
       </c>
       <c r="B107" s="3" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>203-041</t>
+          <t>203-021</t>
         </is>
       </c>
       <c r="B108" s="3" t="n">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>203-042</t>
+          <t>203-022</t>
         </is>
       </c>
       <c r="B109" s="3" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>203-043</t>
+          <t>203-023</t>
         </is>
       </c>
       <c r="B110" s="3" t="n">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>203-044</t>
+          <t>203-024</t>
         </is>
       </c>
       <c r="B111" s="3" t="n">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>203-045</t>
+          <t>203-025</t>
         </is>
       </c>
       <c r="B112" s="3" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>203-046</t>
+          <t>203-026</t>
         </is>
       </c>
       <c r="B113" s="3" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>203-047</t>
+          <t>203-027</t>
         </is>
       </c>
       <c r="B114" s="3" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>203-048</t>
+          <t>203-028</t>
         </is>
       </c>
       <c r="B115" s="3" t="n">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>203-049</t>
+          <t>203-029</t>
         </is>
       </c>
       <c r="B116" s="3" t="n">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>203-050</t>
+          <t>203-030</t>
         </is>
       </c>
       <c r="B117" s="3" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>203-051</t>
+          <t>203-031</t>
         </is>
       </c>
       <c r="B118" s="3" t="n">
@@ -1803,317 +1803,317 @@
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>203-052</t>
+          <t>203-032</t>
         </is>
       </c>
       <c r="B119" s="3" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>203-053</t>
+          <t>203-033</t>
         </is>
       </c>
       <c r="B120" s="3" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>203-054</t>
+          <t>203-034</t>
         </is>
       </c>
       <c r="B121" s="3" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>203-055</t>
+          <t>203-035</t>
         </is>
       </c>
       <c r="B122" s="3" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>203-056</t>
+          <t>203-036</t>
         </is>
       </c>
       <c r="B123" s="3" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>203-057</t>
+          <t>203-037</t>
         </is>
       </c>
       <c r="B124" s="3" t="n">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>203-058</t>
+          <t>203-038</t>
         </is>
       </c>
       <c r="B125" s="3" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>203-059</t>
+          <t>203-039</t>
         </is>
       </c>
       <c r="B126" s="3" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>203-060</t>
+          <t>203-040</t>
         </is>
       </c>
       <c r="B127" s="3" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>203-061</t>
+          <t>203-041</t>
         </is>
       </c>
       <c r="B128" s="3" t="n">
-        <v>6</v>
+        <v>54</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>203-062</t>
+          <t>203-042</t>
         </is>
       </c>
       <c r="B129" s="3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>203-063</t>
+          <t>203-043</t>
         </is>
       </c>
       <c r="B130" s="3" t="n">
-        <v>7</v>
+        <v>57</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>203-064</t>
+          <t>203-044</t>
         </is>
       </c>
       <c r="B131" s="3" t="n">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>204-001</t>
+          <t>203-045</t>
         </is>
       </c>
       <c r="B132" s="3" t="n">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>204-002</t>
+          <t>203-046</t>
         </is>
       </c>
       <c r="B133" s="3" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>205-001</t>
+          <t>203-047</t>
         </is>
       </c>
       <c r="B134" s="3" t="n">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>205-002</t>
+          <t>203-048</t>
         </is>
       </c>
       <c r="B135" s="3" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>205-003</t>
+          <t>203-049</t>
         </is>
       </c>
       <c r="B136" s="3" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>292-001</t>
+          <t>203-050</t>
         </is>
       </c>
       <c r="B137" s="3" t="n">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>292-002</t>
+          <t>203-051</t>
         </is>
       </c>
       <c r="B138" s="3" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>292-003</t>
+          <t>203-052</t>
         </is>
       </c>
       <c r="B139" s="3" t="n">
-        <v>70</v>
+        <v>21</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>292-004</t>
+          <t>203-053</t>
         </is>
       </c>
       <c r="B140" s="3" t="n">
-        <v>58</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>292-005</t>
+          <t>203-054</t>
         </is>
       </c>
       <c r="B141" s="3" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>292-006</t>
+          <t>203-055</t>
         </is>
       </c>
       <c r="B142" s="3" t="n">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>292-007</t>
+          <t>203-056</t>
         </is>
       </c>
       <c r="B143" s="3" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>292-008</t>
+          <t>203-057</t>
         </is>
       </c>
       <c r="B144" s="3" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>292-009</t>
+          <t>203-058</t>
         </is>
       </c>
       <c r="B145" s="3" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>292-010</t>
+          <t>203-059</t>
         </is>
       </c>
       <c r="B146" s="3" t="n">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>292-011</t>
+          <t>203-060</t>
         </is>
       </c>
       <c r="B147" s="3" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>292-012</t>
+          <t>203-061</t>
         </is>
       </c>
       <c r="B148" s="3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>292-013</t>
+          <t>203-062</t>
         </is>
       </c>
       <c r="B149" s="3" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="3" t="inlineStr">
         <is>
-          <t>292-014</t>
+          <t>203-063</t>
         </is>
       </c>
       <c r="B150" s="3" t="n">
@@ -2123,10 +2123,210 @@
     <row r="151">
       <c r="A151" s="3" t="inlineStr">
         <is>
+          <t>203-064</t>
+        </is>
+      </c>
+      <c r="B151" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="3" t="inlineStr">
+        <is>
+          <t>204-001</t>
+        </is>
+      </c>
+      <c r="B152" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="3" t="inlineStr">
+        <is>
+          <t>204-002</t>
+        </is>
+      </c>
+      <c r="B153" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="3" t="inlineStr">
+        <is>
+          <t>205-001</t>
+        </is>
+      </c>
+      <c r="B154" s="3" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="3" t="inlineStr">
+        <is>
+          <t>205-002</t>
+        </is>
+      </c>
+      <c r="B155" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="3" t="inlineStr">
+        <is>
+          <t>205-003</t>
+        </is>
+      </c>
+      <c r="B156" s="3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="3" t="inlineStr">
+        <is>
+          <t>292-001</t>
+        </is>
+      </c>
+      <c r="B157" s="3" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="3" t="inlineStr">
+        <is>
+          <t>292-002</t>
+        </is>
+      </c>
+      <c r="B158" s="3" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="3" t="inlineStr">
+        <is>
+          <t>292-003</t>
+        </is>
+      </c>
+      <c r="B159" s="3" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="3" t="inlineStr">
+        <is>
+          <t>292-004</t>
+        </is>
+      </c>
+      <c r="B160" s="3" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="3" t="inlineStr">
+        <is>
+          <t>292-005</t>
+        </is>
+      </c>
+      <c r="B161" s="3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="3" t="inlineStr">
+        <is>
+          <t>292-006</t>
+        </is>
+      </c>
+      <c r="B162" s="3" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="3" t="inlineStr">
+        <is>
+          <t>292-007</t>
+        </is>
+      </c>
+      <c r="B163" s="3" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="3" t="inlineStr">
+        <is>
+          <t>292-008</t>
+        </is>
+      </c>
+      <c r="B164" s="3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="3" t="inlineStr">
+        <is>
+          <t>292-009</t>
+        </is>
+      </c>
+      <c r="B165" s="3" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="3" t="inlineStr">
+        <is>
+          <t>292-010</t>
+        </is>
+      </c>
+      <c r="B166" s="3" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="3" t="inlineStr">
+        <is>
+          <t>292-011</t>
+        </is>
+      </c>
+      <c r="B167" s="3" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="3" t="inlineStr">
+        <is>
+          <t>292-012</t>
+        </is>
+      </c>
+      <c r="B168" s="3" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="3" t="inlineStr">
+        <is>
+          <t>292-013</t>
+        </is>
+      </c>
+      <c r="B169" s="3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="3" t="inlineStr">
+        <is>
+          <t>292-014</t>
+        </is>
+      </c>
+      <c r="B170" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="3" t="inlineStr">
+        <is>
           <t>292-015</t>
         </is>
       </c>
-      <c r="B151" s="3" t="n">
+      <c r="B171" s="3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2214,10 +2414,10 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>302</v>
+        <v>363</v>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
@@ -2232,10 +2432,10 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>365</v>
+        <v>410</v>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
@@ -2286,10 +2486,10 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>1183</v>
+        <v>1289</v>
       </c>
       <c r="D8" s="3" t="n"/>
     </row>
@@ -2304,7 +2504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2591,7 +2791,7 @@
         </is>
       </c>
       <c r="B28" s="3" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29">
@@ -2601,7 +2801,7 @@
         </is>
       </c>
       <c r="B29" s="3" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30">
@@ -2611,7 +2811,7 @@
         </is>
       </c>
       <c r="B30" s="3" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -2621,7 +2821,7 @@
         </is>
       </c>
       <c r="B31" s="3" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32">
@@ -2631,7 +2831,7 @@
         </is>
       </c>
       <c r="B32" s="3" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
@@ -2661,7 +2861,7 @@
         </is>
       </c>
       <c r="B35" s="3" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36">
@@ -2671,7 +2871,7 @@
         </is>
       </c>
       <c r="B36" s="3" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37">
@@ -2691,7 +2891,7 @@
         </is>
       </c>
       <c r="B38" s="3" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39">
@@ -2707,260 +2907,300 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>209-001</t>
+          <t>208-018</t>
         </is>
       </c>
       <c r="B40" s="3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
         <is>
-          <t>209-002</t>
+          <t>209-001</t>
         </is>
       </c>
       <c r="B41" s="3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>209-006</t>
+          <t>209-002</t>
         </is>
       </c>
       <c r="B42" s="3" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>209-007</t>
+          <t>209-006</t>
         </is>
       </c>
       <c r="B43" s="3" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>209-005</t>
+          <t>209-007</t>
         </is>
       </c>
       <c r="B44" s="3" t="n">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>209-003</t>
+          <t>209-005</t>
         </is>
       </c>
       <c r="B45" s="3" t="n">
-        <v>22</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>209-004</t>
+          <t>209-003</t>
         </is>
       </c>
       <c r="B46" s="3" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>209-008</t>
+          <t>209-004</t>
         </is>
       </c>
       <c r="B47" s="3" t="n">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>209-009</t>
+          <t>209-008</t>
         </is>
       </c>
       <c r="B48" s="3" t="n">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>209-012</t>
+          <t>209-009</t>
         </is>
       </c>
       <c r="B49" s="3" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>209-011</t>
+          <t>209-012</t>
         </is>
       </c>
       <c r="B50" s="3" t="n">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>209-013</t>
+          <t>209-011</t>
         </is>
       </c>
       <c r="B51" s="3" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>209-014</t>
+          <t>209-013</t>
         </is>
       </c>
       <c r="B52" s="3" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>209-016</t>
+          <t>209-014</t>
         </is>
       </c>
       <c r="B53" s="3" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>209-015</t>
+          <t>209-016</t>
         </is>
       </c>
       <c r="B54" s="3" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>210-001</t>
+          <t>209-015</t>
         </is>
       </c>
       <c r="B55" s="3" t="n">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>210-002</t>
+          <t>209-018</t>
         </is>
       </c>
       <c r="B56" s="3" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>210-003</t>
+          <t>209-019</t>
         </is>
       </c>
       <c r="B57" s="3" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>210-004</t>
+          <t>209-017</t>
         </is>
       </c>
       <c r="B58" s="3" t="n">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>210-005</t>
+          <t>210-001</t>
         </is>
       </c>
       <c r="B59" s="3" t="n">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>211-001</t>
+          <t>210-002</t>
         </is>
       </c>
       <c r="B60" s="3" t="n">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>211-003</t>
+          <t>210-003</t>
         </is>
       </c>
       <c r="B61" s="3" t="n">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>211-002</t>
+          <t>210-004</t>
         </is>
       </c>
       <c r="B62" s="3" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>211-004</t>
+          <t>210-005</t>
         </is>
       </c>
       <c r="B63" s="3" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>211-005</t>
+          <t>211-001</t>
         </is>
       </c>
       <c r="B64" s="3" t="n">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
+          <t>211-003</t>
+        </is>
+      </c>
+      <c r="B65" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="inlineStr">
+        <is>
+          <t>211-002</t>
+        </is>
+      </c>
+      <c r="B66" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="inlineStr">
+        <is>
+          <t>211-004</t>
+        </is>
+      </c>
+      <c r="B67" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="inlineStr">
+        <is>
+          <t>211-005</t>
+        </is>
+      </c>
+      <c r="B68" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3" t="inlineStr">
+        <is>
           <t>211-006</t>
         </is>
       </c>
-      <c r="B65" s="3" t="n">
+      <c r="B69" s="3" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>